<commit_message>
dependency alerts captued in analysis doc
</commit_message>
<xml_diff>
--- a/ibrowser/docs/Technical Debt.xlsx
+++ b/ibrowser/docs/Technical Debt.xlsx
@@ -3,16 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BED871-C548-4EED-B7D6-59545D59D8A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{25774F0E-F977-45D9-8041-8BD1403884E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="29070" windowHeight="16500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sonar Info And Code Weakness" sheetId="1" r:id="rId1"/>
     <sheet name="cyclic referenece" sheetId="2" r:id="rId2"/>
     <sheet name="Potential Code Vulnerabilities " sheetId="3" r:id="rId3"/>
+    <sheet name="Dependencies Vulnerabilities" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:W14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1282,6 +1284,99 @@
         <a:xfrm>
           <a:off x="333375" y="76200"/>
           <a:ext cx="13142857" cy="8609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>380190</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>46667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E460855-D8B6-4931-BE45-4B1D7EADD822}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6476190" cy="7666667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8707</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>151478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07434A85-6711-48E0-B09C-D71C01709B68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="7829550"/>
+          <a:ext cx="6542857" cy="7371428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7251,7 +7346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD974EE-725B-411C-B5CE-E096A046ECA8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
@@ -7271,4 +7366,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF0454E-10FA-4749-B3F1-59C1A7F9DD95}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>